<commit_message>
watchlist new test cases implementations
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>TCID</t>
   </si>
@@ -176,17 +176,37 @@
     <t>SKIP</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>UnwatchArticleFromSearch</t>
+  </si>
+  <si>
+    <t>To verify that user is able to unwatch a document from search results page</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>To verify that user is able to unwatch a document from document(Record View) page</t>
+  </si>
+  <si>
+    <t>UnwatchArticleFromRecordViewTest</t>
+  </si>
+  <si>
+    <t>To verify that the following fields are getting displayed for each document in watchlist page:
+a)Times cited
+b)Comments
+c)Views</t>
+  </si>
+  <si>
+    <t>WatchlistArticleDocInfoTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -218,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -241,11 +261,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -261,6 +292,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,18 +593,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="105.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="105.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -596,7 +629,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>37</v>
@@ -610,7 +643,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>37</v>
@@ -624,10 +657,52 @@
         <v>36</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="60">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -646,10 +721,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="12.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="52.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="5" width="83.85546875" collapsed="true"/>
-    <col min="4" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="52.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">

</xml_diff>

<commit_message>
Following are the watchlist new script implementation 1)Watchlist Delete Aritcle test 2)watchlist more button valiations, if article count below 10 or above 10 3)navigate from record view page to watchlist page
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
   <si>
     <t>TCID</t>
   </si>
@@ -185,9 +185,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>To verify that user is able to unwatch a document from document(Record View) page</t>
   </si>
   <si>
@@ -201,6 +198,35 @@
   </si>
   <si>
     <t>WatchlistArticleDocInfoTest</t>
+  </si>
+  <si>
+    <t>To verify that document count gets decreased in the watchlist page when a document is deleted from watchlist</t>
+  </si>
+  <si>
+    <t>To verify that MORE button doesn't get displayed if number of documents in watchlist page is less than or equal to 10</t>
+  </si>
+  <si>
+    <t>WatchlistDeleteArticleTest</t>
+  </si>
+  <si>
+    <t>WatchlistMoreButtonBelowTenArticlesTest</t>
+  </si>
+  <si>
+    <t>WatchlistMoreButtonAboveTenArticlesTest</t>
+  </si>
+  <si>
+    <t>NavigateToWatchlistFromRVTest</t>
+  </si>
+  <si>
+    <t>To verify that app navigates to correct page when user navigates back from document page</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify that MORE button is present in watchlist page if total search results is more than 10
+To verify that MORE button is working correctly in watchlist page
+</t>
   </si>
 </sst>
 </file>
@@ -593,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -679,10 +705,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>30</v>
@@ -692,17 +718,73 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="60">
-      <c r="A7" t="s">
-        <v>45</v>
+      <c r="A7" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30">
+      <c r="A9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="61.5" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Running suites e and f
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t>TCID</t>
   </si>
@@ -225,18 +225,11 @@
 To verify that MORE button is working correctly in watchlist page
 </t>
   </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -613,15 +606,15 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="105.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="105.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -660,7 +653,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>37</v>
@@ -674,7 +667,7 @@
         <v>36</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>37</v>
@@ -794,10 +787,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="12.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="52.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="5" width="83.85546875" collapsed="true"/>
-    <col min="4" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="52.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">

</xml_diff>

<commit_message>
Running suites e and f again
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="53">
   <si>
     <t>TCID</t>
   </si>
@@ -230,6 +230,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -611,10 +612,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="105.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="105.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -787,10 +788,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="52.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="12.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="52.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="83.85546875" collapsed="true"/>
+    <col min="4" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">

</xml_diff>

<commit_message>
running  test case from watchlist
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -615,7 +615,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -690,7 +690,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>54</v>
@@ -718,7 +718,7 @@
         <v>43</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>55</v>
@@ -732,7 +732,7 @@
         <v>45</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>55</v>
@@ -746,7 +746,7 @@
         <v>46</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>54</v>
@@ -760,7 +760,7 @@
         <v>52</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>55</v>
@@ -774,7 +774,7 @@
         <v>51</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
code changes are done for watchlist and notification
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
   <si>
     <t>TCID</t>
   </si>
@@ -221,6 +221,15 @@
     <t xml:space="preserve">To verify that MORE button is present in watchlist page if total search results is more than 10
 To verify that MORE button is working correctly in watchlist page
 </t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -604,12 +613,12 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="40.42578125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="105.28515625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
@@ -637,7 +646,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>37</v>
@@ -651,7 +660,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>37</v>
@@ -665,7 +674,7 @@
         <v>36</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>37</v>
@@ -679,7 +688,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>37</v>
@@ -693,7 +702,7 @@
         <v>40</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
         <v>37</v>
@@ -707,7 +716,7 @@
         <v>42</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>37</v>
@@ -721,7 +730,7 @@
         <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>37</v>
@@ -738,7 +747,7 @@
         <v>30</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="61.5" customHeight="1">
@@ -752,7 +761,7 @@
         <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -766,7 +775,7 @@
         <v>30</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in E and F excel files
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14400" windowHeight="10125"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
   <si>
     <t>TCID</t>
   </si>
@@ -155,82 +155,114 @@
     <t>Y</t>
   </si>
   <si>
-    <t>To verify that user is able to add a document to watchlist from search results page</t>
-  </si>
-  <si>
     <t>TestCase_E1</t>
   </si>
   <si>
     <t>TestCase_E2</t>
   </si>
   <si>
-    <t>To verify that user is able to add a document to watchlist from document page</t>
-  </si>
-  <si>
     <t>TestCase_E3</t>
   </si>
   <si>
-    <t>To verify that user is able to delete a document from watchlist</t>
-  </si>
-  <si>
-    <t>SKIP</t>
-  </si>
-  <si>
-    <t>UnwatchArticleFromSearch</t>
-  </si>
-  <si>
-    <t>To verify that user is able to unwatch a document from search results page</t>
-  </si>
-  <si>
-    <t>To verify that user is able to unwatch a document from document(Record View) page</t>
-  </si>
-  <si>
-    <t>UnwatchArticleFromRecordViewTest</t>
-  </si>
-  <si>
-    <t>To verify that the following fields are getting displayed for each document in watchlist page:
+    <t>TestCase_E4</t>
+  </si>
+  <si>
+    <t>TestCase_E5</t>
+  </si>
+  <si>
+    <t>TestCase_E6</t>
+  </si>
+  <si>
+    <t>TestCase_E7</t>
+  </si>
+  <si>
+    <t>TestCase_E8</t>
+  </si>
+  <si>
+    <t>TestCase_E9</t>
+  </si>
+  <si>
+    <t>TestCase_E10</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add a document to watchlist from search results page</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add a document to watchlist from document page</t>
+  </si>
+  <si>
+    <t>Verify that user is able to delete a document from watchlist</t>
+  </si>
+  <si>
+    <t>Verify that user is able to unwatch a document from search results page</t>
+  </si>
+  <si>
+    <t>Verify that user is able to unwatch a document from document(Record View) page</t>
+  </si>
+  <si>
+    <t>Verify that the following fields are getting displayed for each document in watchlist page:
 a)Times cited
 b)Comments
 c)Views</t>
   </si>
   <si>
-    <t>WatchlistArticleDocInfoTest</t>
-  </si>
-  <si>
-    <t>To verify that document count gets decreased in the watchlist page when a document is deleted from watchlist</t>
-  </si>
-  <si>
-    <t>To verify that MORE button doesn't get displayed if number of documents in watchlist page is less than or equal to 10</t>
-  </si>
-  <si>
-    <t>WatchlistDeleteArticleTest</t>
-  </si>
-  <si>
-    <t>WatchlistMoreButtonBelowTenArticlesTest</t>
-  </si>
-  <si>
-    <t>WatchlistMoreButtonAboveTenArticlesTest</t>
-  </si>
-  <si>
-    <t>NavigateToWatchlistFromRVTest</t>
-  </si>
-  <si>
-    <t>To verify that app navigates to correct page when user navigates back from document page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To verify that MORE button is present in watchlist page if total search results is more than 10
-To verify that MORE button is working correctly in watchlist page
+    <t>Verify that document count gets decreased in the watchlist page when a document is deleted from watchlist</t>
+  </si>
+  <si>
+    <t>Verify that MORE button doesn't get displayed if number of documents in watchlist page is less than or equal to 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that MORE button is present in watchlist page if total search results is more than 10
+Verify that MORE button is working correctly in watchlist page
 </t>
   </si>
   <si>
+    <t>Verify that app navigates to correct page when user navigates back from document page</t>
+  </si>
+  <si>
+    <t>Jira id</t>
+  </si>
+  <si>
+    <t>OPQA-256</t>
+  </si>
+  <si>
+    <t>OPQA-259</t>
+  </si>
+  <si>
+    <t>OPQA-260</t>
+  </si>
+  <si>
+    <t>OPQA-261</t>
+  </si>
+  <si>
+    <t>OPQA-262</t>
+  </si>
+  <si>
+    <t>OPQA-264</t>
+  </si>
+  <si>
+    <t>OPQA-265</t>
+  </si>
+  <si>
+    <t>OPQA-267</t>
+  </si>
+  <si>
+    <t>OPQA-268</t>
+  </si>
+  <si>
+    <t>OPQA-269</t>
+  </si>
+  <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>SKIP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -604,172 +636,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="40.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="105.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="105.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60">
+      <c r="A7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="E8" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="E9" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45">
+      <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="B10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="E10" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="B11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="60">
-      <c r="A7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30">
-      <c r="A9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="61.5" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>37</v>
+      <c r="E11" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -788,10 +854,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="12.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="52.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="5" width="83.85546875" collapsed="true"/>
-    <col min="4" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="52.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">

</xml_diff>

<commit_message>
Fixes for watch list test cases(TestCase_E3,TestCase_E4)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14400" windowHeight="10125"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14205" windowHeight="10125"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Case Steps" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
   <si>
     <t>TCID</t>
   </si>
@@ -185,12 +186,6 @@
     <t>TestCase_E10</t>
   </si>
   <si>
-    <t>Verify that user is able to add a document to watchlist from search results page</t>
-  </si>
-  <si>
-    <t>Verify that user is able to add a document to watchlist from document page</t>
-  </si>
-  <si>
     <t>Verify that user is able to delete a document from watchlist</t>
   </si>
   <si>
@@ -253,17 +248,22 @@
     <t>OPQA-269</t>
   </si>
   <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add document to watchlist from ALL content search results page</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add document to watchlist from document page once it is opened from ALL content set results</t>
+  </si>
+  <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>SKIP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -639,17 +639,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="105.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="109.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -657,7 +657,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -674,16 +674,16 @@
         <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -691,16 +691,16 @@
         <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -708,10 +708,10 @@
         <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>30</v>
@@ -725,16 +725,16 @@
         <v>34</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -742,16 +742,16 @@
         <v>35</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60">
@@ -759,16 +759,16 @@
         <v>36</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -776,16 +776,16 @@
         <v>37</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -793,16 +793,16 @@
         <v>38</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45">
@@ -810,16 +810,16 @@
         <v>39</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -827,16 +827,16 @@
         <v>40</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -847,7 +847,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
@@ -855,10 +855,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="12.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="52.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="5" width="83.85546875" collapsed="true"/>
-    <col min="4" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="52.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">

</xml_diff>

<commit_message>
Removing the invalid test cases for watchlist
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14205" windowHeight="10125"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14400" windowHeight="10125"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Case Steps" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>TCID</t>
   </si>
@@ -168,53 +167,6 @@
     <t>TestCase_E4</t>
   </si>
   <si>
-    <t>TestCase_E5</t>
-  </si>
-  <si>
-    <t>TestCase_E6</t>
-  </si>
-  <si>
-    <t>TestCase_E7</t>
-  </si>
-  <si>
-    <t>TestCase_E8</t>
-  </si>
-  <si>
-    <t>TestCase_E9</t>
-  </si>
-  <si>
-    <t>TestCase_E10</t>
-  </si>
-  <si>
-    <t>Verify that user is able to delete a document from watchlist</t>
-  </si>
-  <si>
-    <t>Verify that user is able to unwatch a document from search results page</t>
-  </si>
-  <si>
-    <t>Verify that user is able to unwatch a document from document(Record View) page</t>
-  </si>
-  <si>
-    <t>Verify that the following fields are getting displayed for each document in watchlist page:
-a)Times cited
-b)Comments
-c)Views</t>
-  </si>
-  <si>
-    <t>Verify that document count gets decreased in the watchlist page when a document is deleted from watchlist</t>
-  </si>
-  <si>
-    <t>Verify that MORE button doesn't get displayed if number of documents in watchlist page is less than or equal to 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify that MORE button is present in watchlist page if total search results is more than 10
-Verify that MORE button is working correctly in watchlist page
-</t>
-  </si>
-  <si>
-    <t>Verify that app navigates to correct page when user navigates back from document page</t>
-  </si>
-  <si>
     <t>Jira id</t>
   </si>
   <si>
@@ -230,34 +182,22 @@
     <t>OPQA-261</t>
   </si>
   <si>
-    <t>OPQA-262</t>
-  </si>
-  <si>
-    <t>OPQA-264</t>
-  </si>
-  <si>
-    <t>OPQA-265</t>
-  </si>
-  <si>
-    <t>OPQA-267</t>
-  </si>
-  <si>
-    <t>OPQA-268</t>
-  </si>
-  <si>
-    <t>OPQA-269</t>
+    <t>PASS</t>
   </si>
   <si>
     <t>SKIP</t>
   </si>
   <si>
-    <t>Verify that user is able to add document to watchlist from ALL content search results page</t>
-  </si>
-  <si>
-    <t>Verify that user is able to add document to watchlist from document page once it is opened from ALL content set results</t>
-  </si>
-  <si>
-    <t>FAIL</t>
+    <t>Verify that user is able to watch an Article from ALL content search results page</t>
+  </si>
+  <si>
+    <t>Verify that user is able to watch an Article from Record View page</t>
+  </si>
+  <si>
+    <t>Verify that user is able to unwatch an Article from watchlist page</t>
+  </si>
+  <si>
+    <t>Verify that user is able to unwatch an Article from ALL content search results page</t>
   </si>
 </sst>
 </file>
@@ -637,17 +577,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="109.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="105.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -657,7 +597,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -674,16 +614,16 @@
         <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -691,16 +631,16 @@
         <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -708,16 +648,16 @@
         <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -725,118 +665,16 @@
         <v>34</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60">
-      <c r="A7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="45">
-      <c r="A10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -847,7 +685,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>

</xml_diff>

<commit_message>
Adding new test cases for watch list(TestCase_E5,TestCase_E6)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14400" windowHeight="10125"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14535" windowHeight="10125"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Case Steps" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>TCID</t>
   </si>
@@ -185,19 +186,37 @@
     <t>PASS</t>
   </si>
   <si>
+    <t>Verify that user is able to watch an Article from ALL content search results page</t>
+  </si>
+  <si>
+    <t>Verify that user is able to watch an Article from Record View page</t>
+  </si>
+  <si>
+    <t>Verify that user is able to unwatch an Article from watchlist page</t>
+  </si>
+  <si>
+    <t>Verify that user is able to unwatch an Article from ALL content search results page</t>
+  </si>
+  <si>
     <t>SKIP</t>
   </si>
   <si>
-    <t>Verify that user is able to watch an Article from ALL content search results page</t>
-  </si>
-  <si>
-    <t>Verify that user is able to watch an Article from Record View page</t>
-  </si>
-  <si>
-    <t>Verify that user is able to unwatch an Article from watchlist page</t>
-  </si>
-  <si>
-    <t>Verify that user is able to unwatch an Article from ALL content search results page</t>
+    <t>TestCase_E5</t>
+  </si>
+  <si>
+    <t>TestCase_E6</t>
+  </si>
+  <si>
+    <t>TBD-01</t>
+  </si>
+  <si>
+    <t>TBD-02</t>
+  </si>
+  <si>
+    <t>Verify that user is able to watch an Patent from ALL content search results page</t>
+  </si>
+  <si>
+    <t>Verify that user is able to watch an Post from ALL content search results page</t>
   </si>
 </sst>
 </file>
@@ -577,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -617,13 +636,13 @@
         <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -634,13 +653,13 @@
         <v>37</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -651,13 +670,13 @@
         <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -668,13 +687,47 @@
         <v>39</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -685,7 +738,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>

</xml_diff>

<commit_message>
Fixing issues for TestCase_E5 and TestCase_E6
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>TCID</t>
   </si>
@@ -198,25 +198,22 @@
     <t>Verify that user is able to unwatch an Article from ALL content search results page</t>
   </si>
   <si>
-    <t>SKIP</t>
-  </si>
-  <si>
     <t>TestCase_E5</t>
   </si>
   <si>
     <t>TestCase_E6</t>
   </si>
   <si>
-    <t>TBD-01</t>
-  </si>
-  <si>
-    <t>TBD-02</t>
-  </si>
-  <si>
     <t>Verify that user is able to watch an Patent from ALL content search results page</t>
   </si>
   <si>
     <t>Verify that user is able to watch an Post from ALL content search results page</t>
+  </si>
+  <si>
+    <t>OPQA-262</t>
+  </si>
+  <si>
+    <t>OPQA-264</t>
   </si>
 </sst>
 </file>
@@ -598,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -642,7 +639,7 @@
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -659,7 +656,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -676,7 +673,7 @@
         <v>30</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -693,18 +690,18 @@
         <v>30</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>30</v>
@@ -715,13 +712,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Adding new Test case for Notification OPQA-215
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>TCID</t>
   </si>
@@ -215,12 +215,74 @@
   <si>
     <t>OPQA-264</t>
   </si>
+  <si>
+    <t>TestCase_E7</t>
+  </si>
+  <si>
+    <t>TestCase_E8</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is able to unwatch a Patent from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ALL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> content search results page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is able to unwatch a Post from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ALL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> content search results page</t>
+    </r>
+  </si>
+  <si>
+    <t>OPQA-265</t>
+  </si>
+  <si>
+    <t>OPQA-267</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +297,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -593,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -724,6 +793,40 @@
         <v>30</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new test cases for watchlist(TestCase_E9,TestCase_E10)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14535" windowHeight="10125"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14535" windowHeight="5415"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
   <si>
     <t>TCID</t>
   </si>
@@ -276,6 +276,27 @@
   </si>
   <si>
     <t>OPQA-267</t>
+  </si>
+  <si>
+    <t>TBD-01</t>
+  </si>
+  <si>
+    <t>Verify that user is able to watch an Article from Article content search results page</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>TestCase_E9</t>
+  </si>
+  <si>
+    <t>TestCase_E10</t>
+  </si>
+  <si>
+    <t>Verify that user is able to unwatch an Article from Article content search results page</t>
+  </si>
+  <si>
+    <t>OPQA-268</t>
   </si>
 </sst>
 </file>
@@ -347,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -363,6 +384,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -704,11 +726,11 @@
       <c r="C2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -721,11 +743,11 @@
       <c r="C3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -738,11 +760,11 @@
       <c r="C4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -755,11 +777,11 @@
       <c r="C5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -772,11 +794,11 @@
       <c r="C6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -789,11 +811,11 @@
       <c r="C7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -806,11 +828,11 @@
       <c r="C8" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -823,10 +845,44 @@
       <c r="C9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new test cases for watchlist(TestCase_E11)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14535" windowHeight="5415"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="12630" windowHeight="9795"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
   <si>
     <t>TCID</t>
   </si>
@@ -284,9 +284,6 @@
     <t>Verify that user is able to watch an Article from Article content search results page</t>
   </si>
   <si>
-    <t>SKIP</t>
-  </si>
-  <si>
     <t>TestCase_E9</t>
   </si>
   <si>
@@ -297,6 +294,15 @@
   </si>
   <si>
     <t>OPQA-268</t>
+  </si>
+  <si>
+    <t>TBD-02</t>
+  </si>
+  <si>
+    <t>TestCase_E11</t>
+  </si>
+  <si>
+    <t>Verify that user is able to unwatch an Article from Record View page</t>
   </si>
 </sst>
 </file>
@@ -684,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -730,7 +736,7 @@
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -747,7 +753,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -764,7 +770,7 @@
         <v>30</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -781,7 +787,7 @@
         <v>30</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -798,7 +804,7 @@
         <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -815,7 +821,7 @@
         <v>30</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -832,7 +838,7 @@
         <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -849,15 +855,15 @@
         <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>58</v>
@@ -871,18 +877,35 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding two new Test Cases for Notifications
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14535" windowHeight="10125"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="12630" windowHeight="9795"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
   <si>
     <t>TCID</t>
   </si>
@@ -276,6 +276,33 @@
   </si>
   <si>
     <t>OPQA-267</t>
+  </si>
+  <si>
+    <t>TBD-01</t>
+  </si>
+  <si>
+    <t>Verify that user is able to watch an Article from Article content search results page</t>
+  </si>
+  <si>
+    <t>TestCase_E9</t>
+  </si>
+  <si>
+    <t>TestCase_E10</t>
+  </si>
+  <si>
+    <t>Verify that user is able to unwatch an Article from Article content search results page</t>
+  </si>
+  <si>
+    <t>OPQA-268</t>
+  </si>
+  <si>
+    <t>TBD-02</t>
+  </si>
+  <si>
+    <t>TestCase_E11</t>
+  </si>
+  <si>
+    <t>Verify that user is able to unwatch an Article from Record View page</t>
   </si>
 </sst>
 </file>
@@ -347,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -363,6 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -704,7 +732,7 @@
       <c r="C2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -721,7 +749,7 @@
       <c r="C3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -738,7 +766,7 @@
       <c r="C4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -755,7 +783,7 @@
       <c r="C5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -772,7 +800,7 @@
       <c r="C6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -789,7 +817,7 @@
       <c r="C7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -806,7 +834,7 @@
       <c r="C8" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -823,10 +851,61 @@
       <c r="C9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes for Watch list test cases(TestCase_E1)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="12630" windowHeight="9795"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14175" windowHeight="9795"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>TCID</t>
   </si>
@@ -165,9 +165,6 @@
     <t>TestCase_E3</t>
   </si>
   <si>
-    <t>TestCase_E4</t>
-  </si>
-  <si>
     <t>Jira id</t>
   </si>
   <si>
@@ -180,58 +177,26 @@
     <t>OPQA-260</t>
   </si>
   <si>
-    <t>OPQA-261</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>Verify that user is able to watch an Article from ALL content search results page</t>
-  </si>
-  <si>
-    <t>Verify that user is able to watch an Article from Record View page</t>
-  </si>
-  <si>
-    <t>Verify that user is able to unwatch an Article from watchlist page</t>
-  </si>
-  <si>
-    <t>Verify that user is able to unwatch an Article from ALL content search results page</t>
-  </si>
-  <si>
-    <t>TestCase_E5</t>
-  </si>
-  <si>
-    <t>TestCase_E6</t>
-  </si>
-  <si>
-    <t>Verify that user is able to watch an Patent from ALL content search results page</t>
-  </si>
-  <si>
-    <t>Verify that user is able to watch an Post from ALL content search results page</t>
-  </si>
-  <si>
-    <t>OPQA-262</t>
-  </si>
-  <si>
-    <t>OPQA-264</t>
-  </si>
-  <si>
-    <t>TestCase_E7</t>
-  </si>
-  <si>
-    <t>TestCase_E8</t>
+    <t>N</t>
+  </si>
+  <si>
+    <t>SKIP</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Verify that user is able to unwatch a Patent from </t>
+      <t xml:space="preserve">Verify that user is able to add an Article from </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color indexed="8"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t>ALL</t>
     </r>
@@ -243,20 +208,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> content search results page</t>
+      <t xml:space="preserve"> content search results page to a particular watchlist</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Verify that user is able to unwatch a Post from </t>
+      <t xml:space="preserve">Verify that user is able to add a Patent from </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color indexed="8"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t>ALL</t>
     </r>
@@ -268,48 +234,41 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> content search results page</t>
+      <t xml:space="preserve"> content search results page to a particular watchlist</t>
     </r>
   </si>
   <si>
-    <t>OPQA-265</t>
-  </si>
-  <si>
-    <t>OPQA-267</t>
-  </si>
-  <si>
-    <t>TBD-01</t>
-  </si>
-  <si>
-    <t>Verify that user is able to watch an Article from Article content search results page</t>
-  </si>
-  <si>
-    <t>TestCase_E9</t>
-  </si>
-  <si>
-    <t>TestCase_E10</t>
-  </si>
-  <si>
-    <t>Verify that user is able to unwatch an Article from Article content search results page</t>
-  </si>
-  <si>
-    <t>OPQA-268</t>
-  </si>
-  <si>
-    <t>TBD-02</t>
-  </si>
-  <si>
-    <t>TestCase_E11</t>
-  </si>
-  <si>
-    <t>Verify that user is able to unwatch an Article from Record View page</t>
+    <r>
+      <t xml:space="preserve">Verify that user is able to add a Post from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> content search results page to a particular watchlist</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,15 +284,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,6 +295,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -391,6 +349,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -710,7 +671,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -727,16 +688,16 @@
         <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -744,13 +705,13 @@
         <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>40</v>
@@ -761,154 +722,26 @@
         <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>43</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
+    <row r="5" spans="1:5" customFormat="1"/>
+    <row r="6" spans="1:5" customFormat="1"/>
+    <row r="7" spans="1:5" customFormat="1"/>
+    <row r="8" spans="1:5" customFormat="1"/>
+    <row r="9" spans="1:5" customFormat="1"/>
+    <row r="10" spans="1:5" customFormat="1"/>
+    <row r="11" spans="1:5" customFormat="1"/>
+    <row r="12" spans="1:5" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding test cases for watch list(TestCase_E5,TestCase_E6)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="15150" windowHeight="10125"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14310" windowHeight="5130"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>TCID</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>TestCase_E6</t>
-  </si>
-  <si>
-    <t>SKIP</t>
   </si>
 </sst>
 </file>
@@ -543,7 +540,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -586,7 +583,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -603,7 +600,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -620,7 +617,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5">

</xml_diff>

<commit_message>
Adding test cases for watch lists
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14310" windowHeight="5130"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="15150" windowHeight="10125"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>TCID</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>TestCase_E6</t>
+  </si>
+  <si>
+    <t>SKIP</t>
   </si>
 </sst>
 </file>
@@ -540,7 +543,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -583,7 +586,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -600,7 +603,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -617,7 +620,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5">

</xml_diff>

<commit_message>
Fixing scripts for watch lists(TestCase_E7,TestCase_E8,TestCase_E9,TestCase_E10)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>TCID</t>
   </si>
@@ -159,7 +159,128 @@
     <t>TestCase_E6</t>
   </si>
   <si>
-    <t>SKIP</t>
+    <t>TestCase_E7</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is able to add an Article from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Articles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> content search results page to a particular watchlist</t>
+    </r>
+  </si>
+  <si>
+    <t>OPQA-265</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is able to unwatch an Article from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Articles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> content search results page</t>
+    </r>
+  </si>
+  <si>
+    <t>TestCase_E8</t>
+  </si>
+  <si>
+    <t>OPQA-267</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is able to add an Article from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Record View </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>page to a particular watchlist</t>
+    </r>
+  </si>
+  <si>
+    <t>TestCase_E9</t>
+  </si>
+  <si>
+    <t>OPQA-268</t>
+  </si>
+  <si>
+    <t>TestCase_E10</t>
+  </si>
+  <si>
+    <t>OPQA-269</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is able to unwatch an Article from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Record View</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -540,17 +661,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="92.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="96.5703125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -586,7 +707,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -603,7 +724,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -620,7 +741,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -671,6 +792,74 @@
         <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new test scripts for watch lists
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
   <si>
     <t>TCID</t>
   </si>
@@ -39,9 +39,6 @@
     <t>OPQA-256</t>
   </si>
   <si>
-    <t>Verify that user is able to add an Article from ALL content search results page to a particular watchlist</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -54,18 +51,12 @@
     <t>OPQA-259</t>
   </si>
   <si>
-    <t>Verify that user is able to add a Patent from ALL content search results page to a particular watchlist</t>
-  </si>
-  <si>
     <t>TestCase_E3</t>
   </si>
   <si>
     <t>OPQA-260</t>
   </si>
   <si>
-    <t>Verify that user is able to add a Post from ALL content search results page to a particular watchlist</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Verify that user is able to unwatch an Article from </t>
     </r>
@@ -281,12 +272,224 @@
       </rPr>
       <t xml:space="preserve"> page</t>
     </r>
+  </si>
+  <si>
+    <t>TestCase_E11</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is able to add a Patent from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Patents</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> content search results page to a particular watchlist</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is able to add a Post from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> content search results page to a particular watchlist</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is able to add a Patent from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> content search results page to a particular watchlist</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is able to add an Article from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> content search results page to a particular watchlist</t>
+    </r>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is able to unwatch a Patent from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Patents</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> content search results page</t>
+    </r>
+  </si>
+  <si>
+    <t>OPQA-272</t>
+  </si>
+  <si>
+    <t>OPQA-273</t>
+  </si>
+  <si>
+    <t>TestCase_E12</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is able to add a Patent from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Record View </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>page to a particular watchlist</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is able to unwatch a Patent from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Record View</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page</t>
+    </r>
+  </si>
+  <si>
+    <t>TestCase_E13</t>
+  </si>
+  <si>
+    <t>TestCase_E14</t>
+  </si>
+  <si>
+    <t>OPQA-276</t>
+  </si>
+  <si>
+    <t>OPQA-277</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -661,19 +864,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="96.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="96.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.48828125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -701,166 +904,234 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new test scripts for watch lists(TestCase_E15,TestCase_E16,TestCase_E17,TestCase_E18)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14310" windowHeight="10125"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14175" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>TCID</t>
   </si>
@@ -380,12 +380,6 @@
     </r>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>SKIP</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Verify that user is able to unwatch a Patent from </t>
     </r>
@@ -482,14 +476,134 @@
     <t>OPQA-277</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <r>
+      <t xml:space="preserve">Verify that user is able to add a Post from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Posts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> content search results page to a particular watchlist</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is able to unwatch a Post from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Posts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> content search results page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is able to watch a Post from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Record View </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>page to a particular watchlist</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user is able to unwatch a Post from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Record View</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page</t>
+    </r>
+  </si>
+  <si>
+    <t>OPQA-278</t>
+  </si>
+  <si>
+    <t>OPQA-280</t>
+  </si>
+  <si>
+    <t>OPQA-282</t>
+  </si>
+  <si>
+    <t>OPQA-285</t>
+  </si>
+  <si>
+    <t>TestCase_E15</t>
+  </si>
+  <si>
+    <t>TestCase_E16</t>
+  </si>
+  <si>
+    <t>TestCase_E17</t>
+  </si>
+  <si>
+    <t>TestCase_E18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -864,19 +978,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="96.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.48828125" collapsed="true"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="96.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -907,10 +1021,10 @@
         <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -924,10 +1038,10 @@
         <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -941,10 +1055,10 @@
         <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -958,10 +1072,10 @@
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -975,10 +1089,10 @@
         <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -992,10 +1106,10 @@
         <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1009,10 +1123,10 @@
         <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1026,10 +1140,10 @@
         <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1043,10 +1157,10 @@
         <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1060,10 +1174,10 @@
         <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1071,66 +1185,134 @@
         <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="C14" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new scripts for watch list(TestCase_E22,TestCase_E23,TestCase_E24)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14310" windowHeight="4995"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14175" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
   <si>
     <t>TCID</t>
   </si>
@@ -611,9 +611,6 @@
     <t>OPQA-288</t>
   </si>
   <si>
-    <t>SKIP</t>
-  </si>
-  <si>
     <t>TestCase_E20</t>
   </si>
   <si>
@@ -629,6 +626,33 @@
   </si>
   <si>
     <t>TestCase_E21</t>
+  </si>
+  <si>
+    <t>TestCase_E22</t>
+  </si>
+  <si>
+    <t>Verify that user is able to unwatch an Article from watchlist page</t>
+  </si>
+  <si>
+    <t>OPQA-293</t>
+  </si>
+  <si>
+    <t>Verify that user is able to unwatch a Patent from watchlist page</t>
+  </si>
+  <si>
+    <t>Verify that user is able to unwatch a Post from watchlist page</t>
+  </si>
+  <si>
+    <t>TestCase_E23</t>
+  </si>
+  <si>
+    <t>TestCase_E24</t>
+  </si>
+  <si>
+    <t>OPQA-294</t>
+  </si>
+  <si>
+    <t>OPQA-295</t>
   </si>
 </sst>
 </file>
@@ -1009,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1055,7 +1079,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1072,7 +1096,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1089,7 +1113,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1106,7 +1130,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1123,7 +1147,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1140,7 +1164,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1157,7 +1181,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1174,7 +1198,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1191,7 +1215,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1208,7 +1232,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1225,7 +1249,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1242,7 +1266,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1259,7 +1283,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1276,7 +1300,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1293,7 +1317,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1310,7 +1334,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1327,7 +1351,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1344,7 +1368,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45">
@@ -1361,15 +1385,15 @@
         <v>7</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="45">
       <c r="A21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>62</v>
@@ -1378,23 +1402,74 @@
         <v>7</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="45">
       <c r="A22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="B23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes for watch list test scripts & one new test script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14175" windowHeight="9795"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14310" windowHeight="6525"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="87">
   <si>
     <t>TCID</t>
   </si>
@@ -667,10 +667,19 @@
     <t>TestCase_E26</t>
   </si>
   <si>
-    <t>Verify that user is able to create a new watchlist||Verify that user is able to name the watchlists||Verify that a user can add description to his watchlist</t>
-  </si>
-  <si>
-    <t>OPQA-312 ||OPQA-314 ||OPQA-317</t>
+    <t>OPQA-314 ||OPQA-317</t>
+  </si>
+  <si>
+    <t>OPQA-312</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create a new watchlist</t>
+  </si>
+  <si>
+    <t>Verify that user is able to name the watchlists||Verify that a user can add description to his watchlist</t>
+  </si>
+  <si>
+    <t>TestCase_E27</t>
   </si>
 </sst>
 </file>
@@ -1057,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1514,7 +1523,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="45">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>81</v>
       </c>
@@ -1522,12 +1531,29 @@
         <v>83</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30">
+      <c r="A28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="C28" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new test cases for watchlist(TestCase_E28,TestCase_E29)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14310" windowHeight="6525"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14175" windowHeight="9795"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="93">
   <si>
     <t>TCID</t>
   </si>
@@ -670,16 +670,36 @@
     <t>OPQA-314 ||OPQA-317</t>
   </si>
   <si>
-    <t>OPQA-312</t>
-  </si>
-  <si>
-    <t>Verify that user is able to create a new watchlist</t>
-  </si>
-  <si>
     <t>Verify that user is able to name the watchlists||Verify that a user can add description to his watchlist</t>
   </si>
   <si>
     <t>TestCase_E27</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create multiple watchlists</t>
+  </si>
+  <si>
+    <t>TestCase_E28</t>
+  </si>
+  <si>
+    <t>OPQA-313</t>
+  </si>
+  <si>
+    <t>TestCase_E29</t>
+  </si>
+  <si>
+    <t>OPQA-320
+||OPQA-623</t>
+  </si>
+  <si>
+    <t>Verify that user is able to share watchlist publically||Verify that user is able to see his public watchlists on his own profile page</t>
+  </si>
+  <si>
+    <t>OPQA-312
+||OPQA-624</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create a new watchlist||Verify that user is able to see his private watchlists on his own profile page</t>
   </si>
 </sst>
 </file>
@@ -1066,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1523,15 +1543,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" ht="30">
       <c r="A27" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>7</v>
@@ -1542,18 +1562,52 @@
     </row>
     <row r="28" spans="1:5" ht="30">
       <c r="A28" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>82</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="D29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30">
+      <c r="A30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
code refactoring for watch list test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14310" windowHeight="10125"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14175" windowHeight="5085"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="117">
   <si>
     <t>TCID</t>
   </si>
@@ -764,6 +764,17 @@
   </si>
   <si>
     <t>OPQA-618</t>
+  </si>
+  <si>
+    <t>TestCase_E37</t>
+  </si>
+  <si>
+    <t>Verify that user is able to delete a watchlist||Verify that user is not able to see his watchlist on his own 
+profile page once that particular watchlist is deleted.</t>
+  </si>
+  <si>
+    <t>OPQA-625
+||OPQA-1104</t>
   </si>
 </sst>
 </file>
@@ -1150,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1791,6 +1802,23 @@
         <v>7</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30">
+      <c r="A38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new test case for Notifications
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14310" windowHeight="10125"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14175" windowHeight="5085"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="117">
   <si>
     <t>TCID</t>
   </si>
@@ -764,6 +764,17 @@
   </si>
   <si>
     <t>OPQA-618</t>
+  </si>
+  <si>
+    <t>TestCase_E37</t>
+  </si>
+  <si>
+    <t>Verify that user is able to delete a watchlist||Verify that user is not able to see his watchlist on his own 
+profile page once that particular watchlist is deleted.</t>
+  </si>
+  <si>
+    <t>OPQA-625
+||OPQA-1104</t>
   </si>
 </sst>
 </file>
@@ -1150,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1791,6 +1802,23 @@
         <v>7</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30">
+      <c r="A38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding test case TestCase_E38
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14175" windowHeight="5085"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14175" windowHeight="6285"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="120">
   <si>
     <t>TCID</t>
   </si>
@@ -775,6 +775,15 @@
   <si>
     <t>OPQA-625
 ||OPQA-1104</t>
+  </si>
+  <si>
+    <t>Verify that a user's public watchlist is not visible to another user once that particular watchlist is deleted.</t>
+  </si>
+  <si>
+    <t>TestCase_E38</t>
+  </si>
+  <si>
+    <t>OPQA-1105</t>
   </si>
 </sst>
 </file>
@@ -1161,10 +1170,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1819,6 +1828,23 @@
         <v>7</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding Notification Test Case
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14175" windowHeight="6285"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14310" windowHeight="2520"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="123">
   <si>
     <t>TCID</t>
   </si>
@@ -730,19 +730,7 @@
     <t>OPQA-328</t>
   </si>
   <si>
-    <t>Verify that anyone can see the public watchlists of a user on user's profile page</t>
-  </si>
-  <si>
-    <t>OPQA-321</t>
-  </si>
-  <si>
     <t>TestCase_E33</t>
-  </si>
-  <si>
-    <t>Verify that no one can see the private watchlists of a user on user's profile page</t>
-  </si>
-  <si>
-    <t>OPQA-329</t>
   </si>
   <si>
     <t>TestCase_E34</t>
@@ -784,6 +772,29 @@
   </si>
   <si>
     <t>OPQA-1105</t>
+  </si>
+  <si>
+    <t>Verify that anyone can see the public watchlists of a user on user's profile page||Verify that user1 is able to see a watchlist on user2's profile page,  once user2's private watchlist is made to public.</t>
+  </si>
+  <si>
+    <t>OPQA-321
+||OPQA-621</t>
+  </si>
+  <si>
+    <t>Verify that no one can see the private watchlists of a user on user's profile page||Verify that user1 is not able to see a watchlist on user2's profile page,  once user2's public watchlist is reverted to private.</t>
+  </si>
+  <si>
+    <t>OPQA-329
+||OPQA-621</t>
+  </si>
+  <si>
+    <t>Verify that same article can be added to multiple watchlists</t>
+  </si>
+  <si>
+    <t>TestCase_E39</t>
+  </si>
+  <si>
+    <t>OPQA-1106</t>
   </si>
 </sst>
 </file>
@@ -1170,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1746,32 +1757,32 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" ht="30">
       <c r="A34" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30">
+      <c r="A35" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>106</v>
+      <c r="B35" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>7</v>
@@ -1782,13 +1793,13 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>7</v>
@@ -1799,13 +1810,13 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>7</v>
@@ -1816,13 +1827,13 @@
     </row>
     <row r="38" spans="1:5" ht="30">
       <c r="A38" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>7</v>
@@ -1833,18 +1844,35 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E39" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding TestCase_E43 & fixes for watch list scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14310" windowHeight="10125"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13830" windowHeight="9795"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="135">
   <si>
     <t>TCID</t>
   </si>
@@ -825,6 +825,16 @@
   <si>
     <t>OPQA-298
 ||OPQA-304</t>
+  </si>
+  <si>
+    <t>OPQA-300
+||OPQA-306</t>
+  </si>
+  <si>
+    <t>TestCase_E43</t>
+  </si>
+  <si>
+    <t>Verify that user is able to watch a patent to a particular watchlist from notification in home page||Verify that user is able to unwatch a patent from watchlist from notification in home page</t>
   </si>
 </sst>
 </file>
@@ -1211,10 +1221,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1954,6 +1964,23 @@
         <v>7</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30">
+      <c r="A44" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Watch list test case fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13575" windowHeight="7545"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13575" windowHeight="4905"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="139">
   <si>
     <t>TCID</t>
   </si>
@@ -424,10 +424,6 @@
     <t>TestCase_E29</t>
   </si>
   <si>
-    <t>OPQA-320
-||OPQA-623</t>
-  </si>
-  <si>
     <t>OPQA-312
 ||OPQA-624</t>
   </si>
@@ -552,9 +548,6 @@
   </si>
   <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
   <si>
     <t>N</t>
@@ -845,10 +838,6 @@
 ||Verify that watchlist name is customizable</t>
   </si>
   <si>
-    <t>Verify that user is able to share watchlist publically
-||Verify that user is able to see his public watchlists on his own profile page</t>
-  </si>
-  <si>
     <t>OPQA-324
 ||OPQA-326
 ||OPQA-328</t>
@@ -885,6 +874,16 @@
   <si>
     <t>Verify that user is able to watch a post(user generated content) to a particular watchlist from notification in home page
 ||Verify that user is able to unwatch a post from watchlist from notification in home page</t>
+  </si>
+  <si>
+    <t>OPQA-313
+||OPQA-320
+||OPQA-623</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create multiple watchlists
+||Verify that user is able to share watchlist publically
+||Verify that user is able to see his public watchlists on his own profile page</t>
   </si>
 </sst>
 </file>
@@ -1347,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1382,16 +1381,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
@@ -1399,16 +1398,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
@@ -1416,16 +1415,16 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1439,10 +1438,10 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1456,10 +1455,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1473,10 +1472,10 @@
         <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45">
@@ -1484,16 +1483,16 @@
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1507,10 +1506,10 @@
         <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30">
@@ -1518,16 +1517,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1541,10 +1540,10 @@
         <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45">
@@ -1552,16 +1551,16 @@
         <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1575,10 +1574,10 @@
         <v>27</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30">
@@ -1586,16 +1585,16 @@
         <v>31</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1609,10 +1608,10 @@
         <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45">
@@ -1620,16 +1619,16 @@
         <v>38</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1643,10 +1642,10 @@
         <v>34</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30">
@@ -1654,16 +1653,16 @@
         <v>40</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1677,10 +1676,10 @@
         <v>35</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45">
@@ -1697,7 +1696,7 @@
         <v>6</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="45">
@@ -1714,7 +1713,7 @@
         <v>6</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="45">
@@ -1731,7 +1730,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1745,10 +1744,10 @@
         <v>51</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1762,10 +1761,10 @@
         <v>53</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1779,10 +1778,10 @@
         <v>54</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1792,14 +1791,14 @@
       <c r="B26" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>109</v>
+        <v>6</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30">
@@ -1807,16 +1806,16 @@
         <v>62</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>128</v>
+        <v>68</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>109</v>
+        <v>6</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="45">
@@ -1824,16 +1823,16 @@
         <v>63</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>129</v>
+        <v>73</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>109</v>
+        <v>6</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1843,286 +1842,286 @@
       <c r="B29" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="5" t="s">
         <v>64</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="45">
       <c r="A30" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>130</v>
+        <v>137</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>138</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>109</v>
+        <v>6</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="45">
       <c r="A31" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>132</v>
+        <v>128</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>109</v>
+        <v>6</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C33" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="45">
       <c r="A34" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="45">
       <c r="A35" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="C36" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="C37" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="45">
       <c r="A38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="C38" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="C39" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="30">
       <c r="A40" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="C41" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="C42" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="30">
       <c r="A43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="C43" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30">
       <c r="A44" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="45.75" thickBot="1">
       <c r="A45" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B45" s="11" t="s">
-        <v>106</v>
-      </c>
       <c r="C45" s="12" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing changes for Notifications
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14310" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13830" windowHeight="10125"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="93">
   <si>
     <t>TCID</t>
   </si>
@@ -548,9 +548,6 @@
   </si>
   <si>
     <t>TestCase_E28</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -649,9 +646,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -948,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1359,11 +1354,11 @@
       <c r="B24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>48</v>
@@ -1393,11 +1388,11 @@
       <c r="B26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>48</v>
@@ -1414,7 +1409,7 @@
         <v>41</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>48</v>
@@ -1431,7 +1426,7 @@
         <v>75</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>48</v>
@@ -1448,7 +1443,7 @@
         <v>76</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>48</v>
@@ -1465,7 +1460,7 @@
         <v>77</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Committing changes made to TestBase class
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/E suite.xlsx
+++ b/src/test/resources/xls/E suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13830" windowHeight="10125"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="11895" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -578,7 +578,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -594,12 +594,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,13 +634,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -943,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -980,7 +974,7 @@
       <c r="B2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -997,7 +991,7 @@
       <c r="B3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1014,7 +1008,7 @@
       <c r="B4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1031,7 +1025,7 @@
       <c r="B5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1048,7 +1042,7 @@
       <c r="B6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1065,7 +1059,7 @@
       <c r="B7" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>60</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1082,7 +1076,7 @@
       <c r="B8" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1099,7 +1093,7 @@
       <c r="B9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>64</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1116,7 +1110,7 @@
       <c r="B10" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>66</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1133,7 +1127,7 @@
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1150,7 +1144,7 @@
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1167,7 +1161,7 @@
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1184,7 +1178,7 @@
       <c r="B14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1201,7 +1195,7 @@
       <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>67</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1218,7 +1212,7 @@
       <c r="B16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>68</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1235,7 +1229,7 @@
       <c r="B17" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="5" t="s">
         <v>79</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1252,7 +1246,7 @@
       <c r="B18" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>70</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1269,7 +1263,7 @@
       <c r="B19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1286,7 +1280,7 @@
       <c r="B20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>72</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1303,7 +1297,7 @@
       <c r="B21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1320,7 +1314,7 @@
       <c r="B22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -1337,7 +1331,7 @@
       <c r="B23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="5" t="s">
         <v>73</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1354,7 +1348,7 @@
       <c r="B24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -1371,7 +1365,7 @@
       <c r="B25" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="5" t="s">
         <v>74</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1422,7 +1416,7 @@
       <c r="B28" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1439,7 +1433,7 @@
       <c r="B29" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1456,7 +1450,7 @@
       <c r="B30" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D30" s="1" t="s">

</xml_diff>